<commit_message>
login scenarios with valid and invalid data
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/HerBalanceDataSheetVM.xlsx
+++ b/src/test/resources/testData/HerBalanceDataSheetVM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jayau\OneDrive\Desktop\GIT-MATHU-VIJI-TRIAL\SELENIUM-BDD-CUCUMBER-FRAMEWORK\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C130EAD-E199-4A90-BBEB-F74B8D18EF81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB51610E-13BC-4A1B-88AF-4D5AB866B770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="600" windowWidth="29040" windowHeight="15000" xr2:uid="{FB278731-2016-4648-9D59-7ACA56D0A234}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>username</t>
   </si>
@@ -70,12 +70,6 @@
   </si>
   <si>
     <t>herbal@123</t>
-  </si>
-  <si>
-    <t>" "</t>
-  </si>
-  <si>
-    <t xml:space="preserve">" " </t>
   </si>
   <si>
     <t>scenario</t>
@@ -494,7 +488,7 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,7 +500,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -548,9 +542,7 @@
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="B5" s="1"/>
       <c r="C5" s="5" t="s">
         <v>9</v>
       </c>
@@ -562,20 +554,14 @@
       <c r="B6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>12</v>
-      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>

</xml_diff>